<commit_message>
newest version of excel
</commit_message>
<xml_diff>
--- a/LouisTestFoundation.xlsx
+++ b/LouisTestFoundation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z75"/>
+  <dimension ref="A1:Y75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,25 +536,20 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Tous droits réservés © 2020– Centre québécois de philanthropie</t>
+          <t>Téléc</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Téléc</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Total actif</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Total actif</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Limites géog</t>
         </is>
@@ -581,7 +576,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation  Fondation 8401, rte Trans-Canadienne Saint-Laurent QC H4S1Z1 </t>
+          <t>8401, rte Trans-Canadienne Saint-Laurent QC H4S1Z1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -652,7 +647,6 @@
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -670,12 +664,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Air-Canada,Fondation</t>
+          <t>Air-Canada,</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">7373, boul. de la Côte-Vertu 7373, boul. de la Côte-Vertu Saint-Laurent QC H4S1Z3 </t>
+          <t>7373, boul. de la Côte-Vertu Saint-Laurent QC H4S1Z3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -746,7 +740,6 @@
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -769,7 +762,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>, The, The390 Park Ave, 9th Floor   New YorkNY10022 USA</t>
+          <t>390 Park Ave, 9th Floor New York NY 10022 USA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -836,15 +829,14 @@
         </is>
       </c>
       <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>412-553-4498</t>
         </is>
       </c>
+      <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -867,7 +859,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1115, rue Laurier O.   1115, rue Laurier O.   OutremontQCH2V2L3</t>
+          <t>1115, rue Laurier O. Outremont QC H2V2L3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -934,15 +926,14 @@
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>514-908-1354</t>
         </is>
       </c>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -965,7 +956,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27 Allstate Parkway Ave., Suite 100   27 Allstate Parkway Ave., Suite 100   MarkhamONL3R5P8</t>
+          <t>27 Allstate Parkway Ave., Suite 100 Markham ON L3R5P8</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1040,15 +1031,14 @@
       </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>905-415-4899</t>
         </is>
       </c>
+      <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1064,8 +1054,16 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The American Express Foundation in Canada </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>C/O Amex Bank of Canada P.O. Box  3204  Stn  F Toronto ON M1W3W7</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>A</t>
@@ -1130,15 +1128,10 @@
       </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>C/O Amex Bank of Canada   P.O. Box  3204  Stn  F TorontoONM1W3W7</t>
-        </is>
-      </c>
+      <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1154,8 +1147,16 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Avon pour les femmes du Canada,</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>5500, rte Transcanadienne Pointe-Claire QC H9R1B6</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>B</t>
@@ -1230,17 +1231,12 @@
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fonda5500, rte Transcanadienne   Pointe-ClaireQCH9R1B6</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
           <t>514-630-5439</t>
         </is>
       </c>
+      <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1256,8 +1252,16 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>CIBC Children's Foundation,</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>25 King St. W., 30 th Floor Commerce Court North Toronto ON M5L1A2</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>A</t>
@@ -1332,17 +1336,12 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The25 King St. W., 30 th Floor   Commerce Court North TorontoONM5L1A2</t>
-        </is>
-      </c>
-      <c r="W9" t="inlineStr">
-        <is>
           <t>416-861-3757</t>
         </is>
       </c>
+      <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1365,7 +1364,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>77 King Street West, 10th Floor   77 King Street West, 10th Floor   TD North Tower TorontoONM5K1A2</t>
+          <t>77 King Street West, 10th Floor TD North Tower Toronto ON M5K1A2</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1440,15 +1439,14 @@
       </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr">
+      <c r="V10" t="inlineStr">
         <is>
           <t>416-308-6426</t>
         </is>
       </c>
+      <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1471,7 +1469,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation J.-Armand Fondation J.-Armand1000, av. J.-A. Bombardier   ValcourtQCJ0E2L0</t>
+          <t>1000, av. J.-A. Bombardier Valcourt QC J0E2L0</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1542,15 +1540,14 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr">
+      <c r="V11" t="inlineStr">
         <is>
           <t>450-532-5499</t>
         </is>
       </c>
+      <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1573,7 +1570,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation8500, pl. Marien   MontréalQCH1B5W8</t>
+          <t>8500, pl. Marien Montréal QC H1B5W8</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1640,19 +1637,18 @@
       </c>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>514-648-4252</t>
+        </is>
+      </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>514-648-4252</t>
-        </is>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
           <t>2427</t>
         </is>
       </c>
+      <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1675,7 +1671,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation444, rue Bouvier   QuébecQCG2J1E3</t>
+          <t>444, rue Bouvier Québec QC G2J1E3</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1750,7 +1746,6 @@
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1773,7 +1768,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La Fondation La Fondation189, boul. Hymus, bur. 601   Pointe-ClaireQCH9R1E9</t>
+          <t>189, boul. Hymus, bur. 601 Pointe-Claire QC H9R1E9</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1848,15 +1843,14 @@
       </c>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr">
+      <c r="V14" t="inlineStr">
         <is>
           <t>514-693-6460</t>
         </is>
       </c>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1879,7 +1873,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>285, rue St-Georges   285, rue St-Georges   DrummondvilleQCJ2C4H3</t>
+          <t>285, rue St-Georges Drummondville QC J2C4H3</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1946,15 +1940,14 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr">
+      <c r="V15" t="inlineStr">
         <is>
           <t>819-477-6297</t>
         </is>
       </c>
+      <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1977,7 +1970,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation de Bienfaisance, Fondation de Bienfaisance,Charitable Foundation of Carquest and Worldpac  35 Worcester Road RexdaleONM9W1K9</t>
+          <t>Charitable Foundation of Carquest and Worldpac 35 Worcester Road Rexdale ON M9W1K9</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2040,15 +2033,14 @@
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr">
+      <c r="V16" t="inlineStr">
         <is>
           <t>416-675-1273</t>
         </is>
       </c>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -2071,7 +2063,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation320, rue St-Joseph E., bur. 100   QuébecQCG1K9E7</t>
+          <t>320, rue St-Joseph E., bur. 100 Québec QC G1K9E7</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2142,15 +2134,14 @@
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr">
+      <c r="V17" t="inlineStr">
         <is>
           <t>418-525-0769</t>
         </is>
       </c>
+      <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2173,7 +2164,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La Fondation La Fondation16, rue Sicard, bur. 50  Ste-ThérèseQCJ7E3W7</t>
+          <t>16, rue Sicard, bur. 50 Ste-Thérèse QC J7E3W7</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2248,15 +2239,14 @@
       </c>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr">
+      <c r="V18" t="inlineStr">
         <is>
           <t>450-435-2428</t>
         </is>
       </c>
+      <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2273,11 +2263,7 @@
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Voir : CIBC Children's Foundation, The Voir : CIBC Children's Foundation, The </t>
-        </is>
-      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
@@ -2298,7 +2284,6 @@
       <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
-      <c r="Z19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2321,7 +2306,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fonds des bienfaiteurs de la Fonds des bienfaiteurs de laCentre Leonardo Da Vinci   8370, boul. Lacordaire, bur. 310 St-LéonardQCH1R3Y6</t>
+          <t>Centre Leonardo Da Vinci 8370, boul. Lacordaire, bur. 310 St-Léonard QC H1R3Y6</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2392,15 +2377,14 @@
       </c>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
-      <c r="W20" t="inlineStr">
+      <c r="V20" t="inlineStr">
         <is>
           <t>514-254-4920</t>
         </is>
       </c>
+      <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr"/>
-      <c r="Z20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2423,7 +2407,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>8400, 2e Avenue   8400, 2e Avenue   MontréalQCH1Z4M6</t>
+          <t>8400, 2e Avenue Montréal QC H1Z4M6</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2498,15 +2482,14 @@
       </c>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr">
+      <c r="V21" t="inlineStr">
         <is>
           <t>514-723-8983</t>
         </is>
       </c>
+      <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2529,7 +2512,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>LaLa1275, rue Saint-Antoine O.   MontréalQCH3C5L2</t>
+          <t>La 1275, rue Saint-Antoine O. Montréal QC H3C5L2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2608,15 +2591,14 @@
         </is>
       </c>
       <c r="U22" t="inlineStr"/>
-      <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr">
+      <c r="V22" t="inlineStr">
         <is>
           <t>514-989-2890</t>
         </is>
       </c>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -2639,7 +2621,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation de la Fondation de la3737, rue Sherbrooke Est   MontréalQCH1X3B3</t>
+          <t>3737, rue Sherbrooke Est Montréal QC H1X3B3</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2706,7 +2688,6 @@
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
-      <c r="Z23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2722,8 +2703,16 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Concessionnaires d'automobiles de Montréal,  </t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>La Fondation de la Corporation des 2335, rue Guénette Saint-Laurent QC H4R2E9</t>
+        </is>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>F</t>
@@ -2798,17 +2787,12 @@
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr">
         <is>
-          <t>La Fondation de la Corporation des2335, rue Guénette   Saint-LaurentQCH4R2E9</t>
-        </is>
-      </c>
-      <c r="W24" t="inlineStr">
-        <is>
           <t>514-331-2045</t>
         </is>
       </c>
+      <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
-      <c r="Z24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2826,12 +2810,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Routhier,Fondation Louis-Charles</t>
+          <t>Routhier,</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>9761, boul. des Sciences  9761, boul. des Sciences  MontréalQCH1J0A6</t>
+          <t>9761, boul. des Sciences Montréal QC H1J0A6</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2876,13 +2860,12 @@
       </c>
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr"/>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr">
+      <c r="X25" t="inlineStr">
         <is>
           <t xml:space="preserve"> 226 624 $</t>
         </is>
       </c>
-      <c r="Z25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2898,8 +2881,16 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Desjardins</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>1, Complexe Desjardins, Tour Sud C.P. 7, succ. Desjardins Montréal QC H5B1B2</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>B</t>
@@ -2974,17 +2965,12 @@
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr">
         <is>
-          <t>, Fondation1, Complexe Desjardins, Tour Sud   C.P. 7, succ. Desjardins MontréalQCH5B1B2</t>
-        </is>
-      </c>
-      <c r="W26" t="inlineStr">
-        <is>
           <t>514-281-2391</t>
         </is>
       </c>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -3007,7 +2993,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The The8300, boul. Pie IX   MontréalQCH1Z4E8</t>
+          <t>8300, boul. Pie IX Montréal QC H1Z4E8</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3074,15 +3060,14 @@
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr">
+      <c r="V27" t="inlineStr">
         <is>
           <t>514-593-4828</t>
         </is>
       </c>
+      <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
-      <c r="Z27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -3105,7 +3090,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>C.P. 4471   C.P. 4471   Mont-TremblantQCJ8E1A1</t>
+          <t>C.P. 4471 Mont-Tremblant QC J8E1A1</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3184,7 +3169,6 @@
       <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr"/>
-      <c r="Z28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -3202,12 +3186,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Fondation Bon départde Canadian Tire du Québec</t>
+          <t>Fondation Bon départ</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">189, boul. Hymus, bur. 601 189, boul. Hymus, bur. 601 Pointe-Claire, QC H9R1E9 </t>
+          <t>189, boul. Hymus, bur. 601 Pointe-Claire, QC H9R1E9</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3270,15 +3254,14 @@
           <t xml:space="preserve"> le Québec. </t>
         </is>
       </c>
-      <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr">
+      <c r="V29" t="inlineStr">
         <is>
           <t>514 693.6460 1 855 693.6555</t>
         </is>
       </c>
+      <c r="W29" t="inlineStr"/>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="inlineStr"/>
-      <c r="Z29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -3301,7 +3284,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> a division of Postmedia Network Inc, The a division of Postmedia Network Inc, TheA Division of Southam   1010, rue Ste-Catherine O., bur. 200 MontréalQCH3B5L1</t>
+          <t>A Division of Southam 1010, rue Ste-Catherine O., bur. 200 Montréal QC H3B5L1</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3372,15 +3355,14 @@
       </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
-      <c r="W30" t="inlineStr">
+      <c r="V30" t="inlineStr">
         <is>
           <t>514-987-2600</t>
         </is>
       </c>
+      <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr"/>
-      <c r="Z30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -3403,7 +3385,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The The7333 Mississauga Rd North   MississaugaONL5N6L4</t>
+          <t>7333 Mississauga Rd North Mississauga ON L5N6L4</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3474,15 +3456,14 @@
       </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
-      <c r="V31" t="inlineStr"/>
-      <c r="W31" t="inlineStr">
+      <c r="V31" t="inlineStr">
         <is>
           <t>905-819-3348</t>
         </is>
       </c>
+      <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="inlineStr"/>
-      <c r="Z31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -3505,7 +3486,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The The1 Concorde Gate, Suite 900   TorontoONM3C4H9</t>
+          <t>1 Concorde Gate, Suite 900 Toronto ON M3C4H9</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3580,15 +3561,14 @@
       </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
-      <c r="V32" t="inlineStr"/>
-      <c r="W32" t="inlineStr">
+      <c r="V32" t="inlineStr">
         <is>
           <t>416-412-6792</t>
         </is>
       </c>
+      <c r="W32" t="inlineStr"/>
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="inlineStr"/>
-      <c r="Z32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -3611,7 +3591,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>180 Honda boul.   180 Honda boul.   MarkhamONL6C0H9</t>
+          <t>180 Honda boul. Markham ON L6C0H9</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3686,15 +3666,14 @@
       </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
-      <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr">
+      <c r="V33" t="inlineStr">
         <is>
           <t>416-865-7048</t>
         </is>
       </c>
+      <c r="W33" t="inlineStr"/>
       <c r="X33" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
-      <c r="Z33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -3717,7 +3696,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation75, boul. René-Lévesque O., 2ième étage   MontréalQCH2Z1A4</t>
+          <t>75, boul. René-Lévesque O., 2ième étage Montréal QC H2Z1A4</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3792,15 +3771,14 @@
       </c>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
-      <c r="V34" t="inlineStr"/>
-      <c r="W34" t="inlineStr">
+      <c r="V34" t="inlineStr">
         <is>
           <t>514-289-2840</t>
         </is>
       </c>
+      <c r="W34" t="inlineStr"/>
       <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr"/>
-      <c r="Z34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -3818,12 +3796,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>La Fondation IKEA,Stichting IKEA Foundation</t>
+          <t>La Fondation IKEA,</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">P.O. Box 11 134 P.O. Box 11 134 2301 EC Leiden The Netherlands </t>
+          <t>P.O. Box 11 134 2301 EC Leiden The Netherlands</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3870,7 +3848,6 @@
       <c r="W35" t="inlineStr"/>
       <c r="X35" t="inlineStr"/>
       <c r="Y35" t="inlineStr"/>
-      <c r="Z35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -3893,7 +3870,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>700, University Ave, bur. 1500   700, University Ave, bur. 1500   TorontoONM5G0A1</t>
+          <t>700, University Ave, bur. 1500 Toronto ON M5G0A1</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3964,15 +3941,14 @@
       </c>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
-      <c r="V36" t="inlineStr"/>
-      <c r="W36" t="inlineStr">
+      <c r="V36" t="inlineStr">
         <is>
           <t>416-440-8970</t>
         </is>
       </c>
+      <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
-      <c r="Z36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -3995,7 +3971,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation  Fondation des Donateurs Jarislowsky Fraser1010, rue Sherbrooke O., bur. 2005   MontréalQCH3A2R7</t>
+          <t>des Donateurs Jarislowsky Fraser 1010, rue Sherbrooke O., bur. 2005 Montréal QC H3A2R7</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4070,15 +4046,14 @@
       </c>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
-      <c r="V37" t="inlineStr"/>
-      <c r="W37" t="inlineStr">
+      <c r="V37" t="inlineStr">
         <is>
           <t>514-842-1882</t>
         </is>
       </c>
+      <c r="W37" t="inlineStr"/>
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr"/>
-      <c r="Z37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -4101,7 +4076,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La Fondation Marcelle et Jean La Fondation Marcelle et Jean1374, av. du Mont-Royal E., bur. 104   MontréalQCH2J1Y7</t>
+          <t>1374, av. du Mont-Royal E., bur. 104 Montréal QC H2J1Y7</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4172,15 +4147,14 @@
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr"/>
-      <c r="W38" t="inlineStr">
+      <c r="V38" t="inlineStr">
         <is>
           <t>514-527-4917</t>
         </is>
       </c>
+      <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr"/>
-      <c r="Z38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -4203,7 +4177,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La Fondation La Fondation393 University Ave, Suite 1100   TorontoONM5G2N9</t>
+          <t>393 University Ave, Suite 1100 Toronto ON M5G2N9</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4278,15 +4252,14 @@
       </c>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
-      <c r="V39" t="inlineStr"/>
-      <c r="W39" t="inlineStr">
+      <c r="V39" t="inlineStr">
         <is>
           <t>416-777-8096</t>
         </is>
       </c>
+      <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr"/>
-      <c r="Z39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -4302,8 +4275,16 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Fondation L’Oréal Canada</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>1500, Boul. Robert-Bourassa, bur. 600 Montréal QC  H3A3S8</t>
+        </is>
+      </c>
       <c r="F40" t="inlineStr">
         <is>
           <t xml:space="preserve">F  </t>
@@ -4344,15 +4325,10 @@
           <t xml:space="preserve"> internationales. </t>
         </is>
       </c>
-      <c r="V40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1500, Boul. Robert-Bourassa, bur. 600  Montréal QC  H3A3S8   </t>
-        </is>
-      </c>
+      <c r="V40" t="inlineStr"/>
       <c r="W40" t="inlineStr"/>
       <c r="X40" t="inlineStr"/>
       <c r="Y40" t="inlineStr"/>
-      <c r="Z40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -4375,7 +4351,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">625, rue Jacques-Parizeau, C.P. 16 040  625, rue Jacques-Parizeau, C.P. 16 040  Québec QC  G1R2G5   </t>
+          <t>625, rue Jacques-Parizeau, C.P. 16 040 Québec QC  G1R2G5</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4422,7 +4398,6 @@
       <c r="W41" t="inlineStr"/>
       <c r="X41" t="inlineStr"/>
       <c r="Y41" t="inlineStr"/>
-      <c r="Z41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -4445,7 +4420,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2159, rue Ste-Catherine Est   2159, rue Ste-Catherine Est   MontréalQCH2K2H9</t>
+          <t>2159, rue Ste-Catherine Est Montréal QC H2K2H9</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4520,15 +4495,14 @@
       </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
-      <c r="V42" t="inlineStr"/>
-      <c r="W42" t="inlineStr">
+      <c r="V42" t="inlineStr">
         <is>
           <t>514-524-5081</t>
         </is>
       </c>
+      <c r="W42" t="inlineStr"/>
       <c r="X42" t="inlineStr"/>
       <c r="Y42" t="inlineStr"/>
-      <c r="Z42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -4551,7 +4525,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Annette Fondation Annette54, rue Amyot   Rivière-du-LoupQCG5R3E9</t>
+          <t>54, rue Amyot Rivière-du-Loup QC G5R3E9</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4614,15 +4588,14 @@
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
-      <c r="V43" t="inlineStr"/>
-      <c r="W43" t="inlineStr">
+      <c r="V43" t="inlineStr">
         <is>
           <t>418-862-5054</t>
         </is>
       </c>
+      <c r="W43" t="inlineStr"/>
       <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
-      <c r="Z43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -4640,12 +4613,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Fondation Raymond James CanadaFoundation</t>
+          <t>Fondation Raymond James Canada</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">2100 – 925 West Georgia Street 2100 – 925 West Georgia Street Vancouver, BC V6C3L2 </t>
+          <t>2100 – 925 West Georgia Street Vancouver, BC V6C3L2</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4708,7 +4681,6 @@
       <c r="W44" t="inlineStr"/>
       <c r="X44" t="inlineStr"/>
       <c r="Y44" t="inlineStr"/>
-      <c r="Z44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -4731,7 +4703,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>180 Queen St. W., Suite 1600   180 Queen St. W., Suite 1600   TorontoONM5V3K1</t>
+          <t>180 Queen St. W., Suite 1600 Toronto ON M5V3K1</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4802,15 +4774,14 @@
       </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
-      <c r="V45" t="inlineStr"/>
-      <c r="W45" t="inlineStr">
+      <c r="V45" t="inlineStr">
         <is>
           <t>866-766-6623</t>
         </is>
       </c>
+      <c r="W45" t="inlineStr"/>
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="inlineStr"/>
-      <c r="Z45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -4833,7 +4804,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Harrison Harrison8800 Main Street   Florenceville-BristolNBE7L1B2</t>
+          <t>8800 Main Street Florenceville-Bristol NB E7L1B2</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4900,15 +4871,14 @@
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr"/>
-      <c r="W46" t="inlineStr">
+      <c r="V46" t="inlineStr">
         <is>
           <t>506-392-0816</t>
         </is>
       </c>
+      <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr"/>
       <c r="Y46" t="inlineStr"/>
-      <c r="Z46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -4924,8 +4894,16 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">McCarthy Tétrault Foundation </t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Toronto Dominion Bank Tower, Suite 5300 P.O. Box 48 Toronto ON M5K1E6</t>
+        </is>
+      </c>
       <c r="F47" t="inlineStr">
         <is>
           <t>B</t>
@@ -4992,17 +4970,12 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr">
         <is>
-          <t>Toronto Dominion Bank Tower, Suite 5300   P.O. Box 48 TorontoONM5K1E6</t>
-        </is>
-      </c>
-      <c r="W47" t="inlineStr">
-        <is>
           <t>416-868-0673</t>
         </is>
       </c>
+      <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr"/>
-      <c r="Z47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -5025,7 +4998,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La Fondation La Fondation8625, rte Transcanadienne   Saint-LaurentQCH4S1Z6</t>
+          <t>8625, rte Transcanadienne Saint-Laurent QC H4S1Z6</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5088,15 +5061,14 @@
       </c>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr"/>
-      <c r="V48" t="inlineStr"/>
-      <c r="W48" t="inlineStr">
+      <c r="V48" t="inlineStr">
         <is>
           <t>514-745-2300</t>
         </is>
       </c>
+      <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr"/>
       <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -5119,7 +5091,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation2500, boul. Daniel-Johnson, 7 étage   LavalQCH7T2P6</t>
+          <t>2500, boul. Daniel-Johnson, 7 étage Laval QC H7T2P6</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5178,15 +5150,14 @@
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
-      <c r="V49" t="inlineStr"/>
-      <c r="W49" t="inlineStr">
+      <c r="V49" t="inlineStr">
         <is>
           <t>450-688-3900</t>
         </is>
       </c>
+      <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
       <c r="Y49" t="inlineStr"/>
-      <c r="Z49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -5209,7 +5180,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">a/s 2500, boul. Daniel-Johnson, bur. 500  a/s 2500, boul. Daniel-Johnson, bur. 500  Laval QC  H7P2T6   </t>
+          <t>a/s 2500, boul. Daniel-Johnson, bur. 500 Laval QC  H7P2T6</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5264,7 +5235,6 @@
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr"/>
       <c r="Y50" t="inlineStr"/>
-      <c r="Z50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -5287,7 +5257,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Thec/o Mitsui &amp; Co. (Canada)   66 Wellington Street West, Suite 3510 TorontoONM5C2T6</t>
+          <t>c/o Mitsui &amp; Co. (Canada) 66 Wellington Street West, Suite 3510 Toronto ON M5C2T6</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5354,15 +5324,14 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr"/>
-      <c r="W51" t="inlineStr">
+      <c r="V51" t="inlineStr">
         <is>
           <t>416-865-1486</t>
         </is>
       </c>
+      <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr"/>
       <c r="Y51" t="inlineStr"/>
-      <c r="Z51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -5385,7 +5354,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La Fondation La Fondation1555, rue Notre-Dame Est   MontréalQCH2L2R5</t>
+          <t>1555, rue Notre-Dame Est Montréal QC H2L2R5</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -5452,15 +5421,14 @@
       <c r="S52" t="inlineStr"/>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
-      <c r="V52" t="inlineStr"/>
-      <c r="W52" t="inlineStr">
+      <c r="V52" t="inlineStr">
         <is>
           <t>514-599-5396</t>
         </is>
       </c>
+      <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr"/>
       <c r="Y52" t="inlineStr"/>
-      <c r="Z52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -5483,7 +5451,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation1000, ch. des Voyageurs   Mont-TremblantQCJ8E1T1</t>
+          <t>1000, ch. des Voyageurs Mont-Tremblant QC J8E1T1</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -5550,15 +5518,14 @@
       </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
-      <c r="V53" t="inlineStr"/>
-      <c r="W53" t="inlineStr">
+      <c r="V53" t="inlineStr">
         <is>
           <t>819-681-3000</t>
         </is>
       </c>
+      <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr"/>
       <c r="Y53" t="inlineStr"/>
-      <c r="Z53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -5581,7 +5548,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>246 Post Road E.   246 Post Road E.   WestportCT06880-3615 USA</t>
+          <t>246 Post Road E. Westport CT 06880-3615 USA</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5652,7 +5619,6 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr"/>
       <c r="Y54" t="inlineStr"/>
-      <c r="Z54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -5670,7 +5636,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Novartis International AG Postfach 4002Basel, Switzerland</t>
+          <t xml:space="preserve">Novartis International AG </t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
@@ -5718,7 +5684,6 @@
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr"/>
       <c r="Y55" t="inlineStr"/>
-      <c r="Z55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -5741,7 +5706,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>c/o Pricewaterhouse Coopers   c/o Pricewaterhouse Coopers   99 Bank Street, Suite 800 OttawaONK1P1K6</t>
+          <t>c/o Pricewaterhouse Coopers 99 Bank Street, Suite 800 Ottawa ON K1P1K6</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5804,15 +5769,14 @@
       <c r="S56" t="inlineStr"/>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
-      <c r="V56" t="inlineStr"/>
-      <c r="W56" t="inlineStr">
+      <c r="V56" t="inlineStr">
         <is>
           <t>613-237-3963</t>
         </is>
       </c>
+      <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr"/>
       <c r="Y56" t="inlineStr"/>
-      <c r="Z56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -5830,12 +5794,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Fondation Loblaw Companies Limited of Canada,Foundation</t>
+          <t>Fondation Loblaw Companies Limited of Canada</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">a/s 400, ave Ste-Croix  a/s 400, ave Ste-Croix  Saint-Laurent QC  H4N3L4   </t>
+          <t>a/s 400, ave Ste-Croix Saint-Laurent QC  H4N3L4</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5882,7 +5846,6 @@
       <c r="W57" t="inlineStr"/>
       <c r="X57" t="inlineStr"/>
       <c r="Y57" t="inlineStr"/>
-      <c r="Z57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -5905,7 +5868,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>155 Wellington Street West, 18th Floor   155 Wellington Street West, 18th Floor   TorontoONM5V3K7</t>
+          <t>155 Wellington Street West, 18th Floor Toronto ON M5V3K7</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5980,15 +5943,14 @@
       </c>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
-      <c r="V58" t="inlineStr"/>
-      <c r="W58" t="inlineStr">
+      <c r="V58" t="inlineStr">
         <is>
           <t>416-974-0624</t>
         </is>
       </c>
+      <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr"/>
       <c r="Y58" t="inlineStr"/>
-      <c r="Z58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -6011,7 +5973,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>100-10 760 Shellbridge Way   100-10 760 Shellbridge Way   RichmondBCV6X3H1</t>
+          <t>100-10 760 Shellbridge Way Richmond BC V6X3H1</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -6086,15 +6048,14 @@
       </c>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
-      <c r="V59" t="inlineStr"/>
-      <c r="W59" t="inlineStr">
+      <c r="V59" t="inlineStr">
         <is>
           <t>604-270-4168</t>
         </is>
       </c>
+      <c r="W59" t="inlineStr"/>
       <c r="X59" t="inlineStr"/>
       <c r="Y59" t="inlineStr"/>
-      <c r="Z59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -6117,7 +6078,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>a/s Les Restaurants Ronald McDonald du Canada   a/s Les Restaurants Ronald McDonald du Canada   1, McDonald's Place TorontoONM3C3L4</t>
+          <t>a/s Les Restaurants Ronald McDonald du Canada 1, McDonald's Place Toronto ON M3C3L4</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6192,15 +6153,14 @@
       </c>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
-      <c r="V60" t="inlineStr"/>
-      <c r="W60" t="inlineStr">
+      <c r="V60" t="inlineStr">
         <is>
           <t>416-446-4679</t>
         </is>
       </c>
+      <c r="W60" t="inlineStr"/>
       <c r="X60" t="inlineStr"/>
       <c r="Y60" t="inlineStr"/>
-      <c r="Z60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -6223,7 +6183,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The The39 Wynford Drive   TorontoONM3C3K5</t>
+          <t>39 Wynford Drive Toronto ON M3C3K5</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -6298,15 +6258,14 @@
       </c>
       <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
-      <c r="V61" t="inlineStr"/>
-      <c r="W61" t="inlineStr">
+      <c r="V61" t="inlineStr">
         <is>
           <t>416-510-5856</t>
         </is>
       </c>
+      <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
-      <c r="Z61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -6329,7 +6288,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation2150, boul. St-Elzéar O.   LavalQCH7L4A8</t>
+          <t>2150, boul. St-Elzéar O. Laval QC H7L4A8</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -6392,19 +6351,18 @@
         </is>
       </c>
       <c r="U62" t="inlineStr"/>
-      <c r="V62" t="inlineStr"/>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>514-856-8706</t>
+        </is>
+      </c>
       <c r="W62" t="inlineStr">
         <is>
-          <t>514-856-8706</t>
-        </is>
-      </c>
-      <c r="X62" t="inlineStr">
-        <is>
           <t>63700</t>
         </is>
       </c>
+      <c r="X62" t="inlineStr"/>
       <c r="Y62" t="inlineStr"/>
-      <c r="Z62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -6427,7 +6385,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation6869, boul. Métropolitain Est   St-LéonardQCH1P1X8</t>
+          <t>6869, boul. Métropolitain Est St-Léonard QC H1P1X8</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -6498,15 +6456,14 @@
       </c>
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr"/>
-      <c r="V63" t="inlineStr"/>
-      <c r="W63" t="inlineStr">
+      <c r="V63" t="inlineStr">
         <is>
           <t>514-328-3375</t>
         </is>
       </c>
+      <c r="W63" t="inlineStr"/>
       <c r="X63" t="inlineStr"/>
       <c r="Y63" t="inlineStr"/>
-      <c r="Z63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -6529,7 +6486,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation du Fondation du1100, boul. René-Lévesque O., 9e étage   MontréalQCH3B5H5</t>
+          <t>1100, boul. René-Lévesque O., 9e étage Montréal QC H3B5H5</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -6600,15 +6557,14 @@
       </c>
       <c r="T64" t="inlineStr"/>
       <c r="U64" t="inlineStr"/>
-      <c r="V64" t="inlineStr"/>
-      <c r="W64" t="inlineStr">
+      <c r="V64" t="inlineStr">
         <is>
           <t>514-940-7342</t>
         </is>
       </c>
+      <c r="W64" t="inlineStr"/>
       <c r="X64" t="inlineStr"/>
       <c r="Y64" t="inlineStr"/>
-      <c r="Z64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -6631,7 +6587,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sodexo Canada Sodexo Canada 5420 North Service Road, Suite 501  Burlington, ON L7L6C7 </t>
+          <t>Sodexo Canada 5420 North Service Road, Suite 501 Burlington, ON L7L6C7</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -6676,7 +6632,7 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>31 décembreAlimentation (santé; dans les écoles). Banques alimentaires (communautaire et vestimentaires, auberges). Éducation (améliorer l’alimentation). Enfants (développement et bien-être). Environnement. Pauvreté. Santé. Services sociaux.</t>
+          <t>31 décembreAlimentation (santé; dans les écoles). Banques alimentaires (communautaire et vestimentaires, auberges). Éducation (améliorer l’alimentation). Enfants (développement et bien-être). Environnement. Pauvreté. Santé. Services sociaux.Activité bénéfice annuelle (ventes aux enchères, tirages, loteries, soirées-bénéfice, galas ou concerts, dons de sociétés et commandites ciblés). Dons jumelés (avec les employés).</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
@@ -6706,15 +6662,10 @@
       </c>
       <c r="T65" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
-      <c r="V65" t="inlineStr">
-        <is>
-          <t>Activité bénéfice annuelle (ventes aux enchères, tirages, loteries, soirées-bénéfice, galas ou concerts, dons de sociétés et commandites ciblés). Dons jumelés (avec les employés).</t>
-        </is>
-      </c>
+      <c r="V65" t="inlineStr"/>
       <c r="W65" t="inlineStr"/>
       <c r="X65" t="inlineStr"/>
       <c r="Y65" t="inlineStr"/>
-      <c r="Z65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -6737,7 +6688,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>c/o Sony of Canada   c/o Sony of Canada   115 Gordon Baker Rd TorontoONM2H3R6</t>
+          <t>c/o Sony of Canada 115 Gordon Baker Rd Toronto ON M2H3R6</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6812,15 +6763,14 @@
       </c>
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
-      <c r="V66" t="inlineStr"/>
-      <c r="W66" t="inlineStr">
+      <c r="V66" t="inlineStr">
         <is>
           <t>416-491-7560</t>
         </is>
       </c>
+      <c r="W66" t="inlineStr"/>
       <c r="X66" t="inlineStr"/>
       <c r="Y66" t="inlineStr"/>
-      <c r="Z66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -6843,7 +6793,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation Fondation2525, boul. Laurier  C.P. 10 500 Ste-FoyQCG1V4L2</t>
+          <t>2525, boul. Laurier  C.P. 10 500 Ste-Foy QC G1V4L2</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6914,15 +6864,14 @@
       </c>
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
-      <c r="V67" t="inlineStr"/>
-      <c r="W67" t="inlineStr">
+      <c r="V67" t="inlineStr">
         <is>
           <t>418-652-1659</t>
         </is>
       </c>
+      <c r="W67" t="inlineStr"/>
       <c r="X67" t="inlineStr"/>
       <c r="Y67" t="inlineStr"/>
-      <c r="Z67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -6941,7 +6890,7 @@
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Voir la Fondation St-Hubert, plus haut. Voir la Fondation St-Hubert, plus haut. </t>
+          <t>Voir la Fondation St-Hubert, plus haut.</t>
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
@@ -6964,7 +6913,6 @@
       <c r="W68" t="inlineStr"/>
       <c r="X68" t="inlineStr"/>
       <c r="Y68" t="inlineStr"/>
-      <c r="Z68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -6987,7 +6935,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t xml:space="preserve">5960 Heisley Rd 5960 Heisley Rd Mentor, OH, 44060-1834  USA </t>
+          <t>5960 Heisley Rd Mentor, OH, 44060-1834  USA</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -7033,8 +6981,7 @@
       <c r="V69" t="inlineStr"/>
       <c r="W69" t="inlineStr"/>
       <c r="X69" t="inlineStr"/>
-      <c r="Y69" t="inlineStr"/>
-      <c r="Z69" t="inlineStr">
+      <c r="Y69" t="inlineStr">
         <is>
           <t>nationales.</t>
         </is>
@@ -7061,7 +7008,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La Fondation pour les enfants La Fondation pour les enfantsRR2, 264 Glen Morris Rd East   St GeorgeONN0E1N0</t>
+          <t>RR2, 264 Glen Morris Rd East St George ON N0E1N0</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -7132,15 +7079,14 @@
       </c>
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
-      <c r="V70" t="inlineStr"/>
-      <c r="W70" t="inlineStr">
+      <c r="V70" t="inlineStr">
         <is>
           <t>519-448-1415</t>
         </is>
       </c>
+      <c r="W70" t="inlineStr"/>
       <c r="X70" t="inlineStr"/>
       <c r="Y70" t="inlineStr"/>
-      <c r="Z70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -7163,7 +7109,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve"> La Fondation La Fondation1155, boul. René-Lévesque O., bur. 3200   MontréalQCH3B0C9</t>
+          <t>1155, boul. René-Lévesque O., bur. 3200 Montréal QC H3B0C9</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -7238,7 +7184,6 @@
       <c r="W71" t="inlineStr"/>
       <c r="X71" t="inlineStr"/>
       <c r="Y71" t="inlineStr"/>
-      <c r="Z71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -7257,7 +7202,7 @@
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">La Fondation Unilever a été révoquée volontairement. La Fondation Unilever a été révoquée volontairement. </t>
+          <t>La Fondation Unilever a été révoquée volontairement.</t>
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
@@ -7280,7 +7225,6 @@
       <c r="W72" t="inlineStr"/>
       <c r="X72" t="inlineStr"/>
       <c r="Y72" t="inlineStr"/>
-      <c r="Z72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -7296,8 +7240,16 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>UPS Foundation,</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>c/o UPS Canada Ltd 6285 Northam Drive, Suite 400 Mississauga ON L4V1X5</t>
+        </is>
+      </c>
       <c r="F73" t="inlineStr">
         <is>
           <t>A</t>
@@ -7366,15 +7318,10 @@
         </is>
       </c>
       <c r="U73" t="inlineStr"/>
-      <c r="V73" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Thec/o UPS Canada Ltd   6285 Northam Drive, Suite 400 MississaugaONL4V1X5</t>
-        </is>
-      </c>
+      <c r="V73" t="inlineStr"/>
       <c r="W73" t="inlineStr"/>
       <c r="X73" t="inlineStr"/>
       <c r="Y73" t="inlineStr"/>
-      <c r="Z73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -7397,7 +7344,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Fondation  Fondation 7007, ch. Côte-de-Liesse   Saint-LaurentQCH4T1G2</t>
+          <t>7007, ch. Côte-de-Liesse Saint-Laurent QC H4T1G2</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -7464,15 +7411,14 @@
       <c r="S74" t="inlineStr"/>
       <c r="T74" t="inlineStr"/>
       <c r="U74" t="inlineStr"/>
-      <c r="V74" t="inlineStr"/>
-      <c r="W74" t="inlineStr">
+      <c r="V74" t="inlineStr">
         <is>
           <t>514-748-9593</t>
         </is>
       </c>
+      <c r="W74" t="inlineStr"/>
       <c r="X74" t="inlineStr"/>
       <c r="Y74" t="inlineStr"/>
-      <c r="Z74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -7495,7 +7441,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The The45 Glover Avenue   P.O. Box 4505 NorwalkCT06856-4505 USA</t>
+          <t>45 Glover Avenue P.O. Box 4505 Norwalk CT 06856-4505 USA</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -7558,15 +7504,14 @@
       </c>
       <c r="T75" t="inlineStr"/>
       <c r="U75" t="inlineStr"/>
-      <c r="V75" t="inlineStr"/>
-      <c r="W75" t="inlineStr">
+      <c r="V75" t="inlineStr">
         <is>
           <t>203-968-3330</t>
         </is>
       </c>
+      <c r="W75" t="inlineStr"/>
       <c r="X75" t="inlineStr"/>
       <c r="Y75" t="inlineStr"/>
-      <c r="Z75" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>